<commit_message>
Adding a zoomed chart of the character flip probability
</commit_message>
<xml_diff>
--- a/content/post/mrz-checksum-failure-analysis/data/mrz_checksum_false_positives.xlsx
+++ b/content/post/mrz-checksum-failure-analysis/data/mrz_checksum_false_positives.xlsx
@@ -223,10 +223,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0767664196413418"/>
-          <c:y val="0.0940788910755541"/>
-          <c:w val="0.898229337557278"/>
-          <c:h val="0.78420467185762"/>
+          <c:x val="0.0767664196413419"/>
+          <c:y val="0.0940361084966202"/>
+          <c:w val="0.898172766872207"/>
+          <c:h val="0.784119106699752"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -596,11 +596,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="32477291"/>
-        <c:axId val="5291032"/>
+        <c:axId val="42776930"/>
+        <c:axId val="20173896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32477291"/>
+        <c:axId val="42776930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -666,13 +666,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5291032"/>
+        <c:crossAx val="20173896"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5291032"/>
+        <c:axId val="20173896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,7 +709,465 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32477291"/>
+        <c:crossAx val="42776930"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0767664196413419"/>
+          <c:y val="0.0940361084966202"/>
+          <c:w val="0.898172766872207"/>
+          <c:h val="0.784119106699752"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>plot!$J$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p_bad_match</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="f58220"/>
+            </a:solidFill>
+            <a:ln w="45720">
+              <a:solidFill>
+                <a:srgbClr val="f58220"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>plot!$B$31:$B$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>plot!$J$31:$J$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.0193647134590669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0172296885368977</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0153935250598347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0138220333172263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0124839772280336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0113508082304527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0103964179373821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00959690994232564</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00893039116032</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00837678308847877</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00791765337074106</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00753606805141597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00721646490211252</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00694454820664518</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.00670720538850502</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00649244586548648</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00628936251605994</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00608811614208</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00587994331241957</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.00565718797211984</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.00541335720164609</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00514320151083954</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.00484282005215509</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.00450979113777514</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.00414332844518954</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.00374446329583152</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.00331625339136</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.00286401839217791</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.00239560272277693</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.00192166598849844</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.00145600138830086</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.00101588250812344</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.000622438879436378</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.000301060687567526</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.18330143956058E-005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="70769968"/>
+        <c:axId val="73214816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="70769968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>p_char</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73214816"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="73214816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="70769968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -770,9 +1228,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>684000</xdr:colOff>
+      <xdr:colOff>683640</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -781,11 +1239,41 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8950680" y="2295000"/>
-        <a:ext cx="6363720" cy="4207320"/>
+        <a:ext cx="6363360" cy="4206960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>802800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>663480</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8930520" y="6674400"/>
+        <a:ext cx="6363360" cy="4206960"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1176,8 +1664,8 @@
   </sheetPr>
   <dimension ref="B2:J66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R48" activeCellId="0" sqref="R48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U44" activeCellId="0" sqref="U44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>